<commit_message>
refine instructions for problem component 2
</commit_message>
<xml_diff>
--- a/INPUT-FILES/homework-input.xlsx
+++ b/INPUT-FILES/homework-input.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,27 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/R/HOMEWORK/INPUT-FILES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF0A0430-E4EF-F745-A25A-A095B8DC382B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DAB379-C936-B243-88ED-849FFFBCD2C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="28340" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="input1" sheetId="1" r:id="rId1"/>
+    <sheet name="input1" sheetId="2" r:id="rId1"/>
+    <sheet name="Input2a" sheetId="3" r:id="rId2"/>
+    <sheet name="Input2b" sheetId="4" r:id="rId3"/>
+    <sheet name="Input2c" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
   <si>
     <t>group</t>
   </si>
   <si>
     <t>score</t>
-  </si>
-  <si>
-    <t>label</t>
   </si>
   <si>
     <t>A</t>
@@ -42,11 +42,23 @@
   <si>
     <t>D</t>
   </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -880,10 +892,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AAA1E7-E49E-C046-8CF3-BEE87EFF0011}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -895,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -906,7 +918,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -917,7 +929,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -928,7 +940,7 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -939,7 +951,7 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -950,7 +962,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -961,7 +973,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -972,7 +984,7 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -983,7 +995,7 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -994,7 +1006,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1005,7 +1017,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1016,7 +1028,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1027,7 +1039,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1038,7 +1050,7 @@
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1049,7 +1061,184 @@
         <v>43</v>
       </c>
       <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866519D9-B9B9-864E-B9BA-4E534680CB9A}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView zoomScale="178" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>6</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38FB1B1E-5523-BA46-AE8A-1993E5ADA581}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F07F055-57C8-4746-975D-F67EC19FBA97}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>